<commit_message>
add BMC check descriptions
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/github/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E29F5D5-329E-FB4F-B7B4-F263F64B1D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AC1EBD-A14A-2A4F-87C6-E58AABC7EFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="262">
   <si>
     <t>Check Type</t>
   </si>
@@ -1105,6 +1105,45 @@
   </si>
   <si>
     <t>counts of visits with visit_concept_id = 9203, visits with conditions with condition_type_concept_id = 2000001280, 2000001281, 2000001282, 2000001283, 2000001284, or 2000001285, and visits that fall into both groups</t>
+  </si>
+  <si>
+    <t>Best Mapped Concepts</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Outpatient Provider Specialty</t>
+  </si>
+  <si>
+    <t>Outpatient Care Site Specialty</t>
+  </si>
+  <si>
+    <t>Outpatient Specialty</t>
+  </si>
+  <si>
+    <t>for inpatient administrations (drug_type_concept_id = 38000180), counts of each RxNorm class to which concepts are mapped</t>
+  </si>
+  <si>
+    <t>for prescription drugs (drug_type_concept_id = 38000177), counts of each RxNorm class to which concepts are mapped</t>
+  </si>
+  <si>
+    <t>counts of each concept_id represented in race_concept_id</t>
+  </si>
+  <si>
+    <t>counts of each concept_id represented in ethnicity_concept_id</t>
+  </si>
+  <si>
+    <t>counts of each unique specialty_concept_id for outpatient providers (visit_concept_id = 9202 when inner joined to visit_occurrence)</t>
+  </si>
+  <si>
+    <t>counts of each unique specialty_concept_id for outpatient care sites (visit_concept_id = 9202 when inner joined to visit_occurrence)</t>
+  </si>
+  <si>
+    <t>counts of each unique specialty_concept_id for outpatient specialties in the specialty table (visit_concept_id = 9202 when inner joined to visit_occurrence)</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1196,6 +1235,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1209,9 +1254,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -1229,6 +1274,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1551,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D147"/>
+  <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2559,102 +2605,102 @@
         <v>171</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>8</v>
+    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>8</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B73" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>174</v>
+        <v>256</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>8</v>
+      <c r="A74" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
-        <v>24</v>
+        <v>250</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>8</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>251</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>8</v>
+        <v>258</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A76" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C76" t="s">
-        <v>30</v>
+        <v>252</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>176</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>8</v>
+      <c r="A77" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C77" t="s">
-        <v>81</v>
+        <v>253</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>8</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A78" s="13" t="s">
+        <v>249</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="C78" t="s">
-        <v>82</v>
+        <v>254</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>178</v>
+        <v>261</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2665,13 +2711,13 @@
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>8</v>
       </c>
@@ -2679,13 +2725,13 @@
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
         <v>8</v>
       </c>
@@ -2693,10 +2739,10 @@
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2704,27 +2750,27 @@
         <v>8</v>
       </c>
       <c r="B82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2732,55 +2778,55 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2788,13 +2834,13 @@
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2805,10 +2851,10 @@
         <v>10</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2819,13 +2865,13 @@
         <v>10</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>8</v>
       </c>
@@ -2833,13 +2879,13 @@
         <v>10</v>
       </c>
       <c r="C91" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>8</v>
       </c>
@@ -2847,10 +2893,10 @@
         <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>80</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2858,27 +2904,27 @@
         <v>8</v>
       </c>
       <c r="B93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C93" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B94" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2886,13 +2932,13 @@
         <v>8</v>
       </c>
       <c r="B95" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2900,13 +2946,13 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C96" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2914,13 +2960,13 @@
         <v>8</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2928,27 +2974,27 @@
         <v>8</v>
       </c>
       <c r="B98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B99" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2959,10 +3005,10 @@
         <v>11</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2973,13 +3019,13 @@
         <v>11</v>
       </c>
       <c r="C101" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>8</v>
       </c>
@@ -2987,10 +3033,10 @@
         <v>11</v>
       </c>
       <c r="C102" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2998,13 +3044,13 @@
         <v>8</v>
       </c>
       <c r="B103" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C103" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3012,27 +3058,27 @@
         <v>8</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C104" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C105" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3040,13 +3086,13 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3054,41 +3100,41 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C107" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B108" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C108" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B109" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C109" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3099,10 +3145,10 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3113,13 +3159,13 @@
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>8</v>
       </c>
@@ -3127,136 +3173,136 @@
         <v>12</v>
       </c>
       <c r="C112" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" s="11" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A113" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B113" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113" t="s">
+        <v>80</v>
+      </c>
+      <c r="D113" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A114" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114" t="s">
+        <v>30</v>
+      </c>
+      <c r="D114" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A115" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B115" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115" t="s">
+        <v>81</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C116" t="s">
+        <v>82</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A117" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B117" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A118" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118" t="s">
+        <v>83</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A119" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B119" t="s">
+        <v>12</v>
+      </c>
+      <c r="C119" t="s">
         <v>84</v>
       </c>
-      <c r="D112" s="11" t="s">
+      <c r="D119" s="11" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B113" t="s">
-        <v>20</v>
-      </c>
-      <c r="C113" t="s">
-        <v>28</v>
-      </c>
-      <c r="D113" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" t="s">
-        <v>20</v>
-      </c>
-      <c r="C114" t="s">
-        <v>89</v>
-      </c>
-      <c r="D114" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B115" t="s">
-        <v>51</v>
-      </c>
-      <c r="C115" t="s">
-        <v>90</v>
-      </c>
-      <c r="D115" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B116" t="s">
-        <v>21</v>
-      </c>
-      <c r="C116" t="s">
-        <v>9</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B117" t="s">
-        <v>21</v>
-      </c>
-      <c r="C117" t="s">
-        <v>41</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B118" t="s">
-        <v>21</v>
-      </c>
-      <c r="C118" t="s">
-        <v>42</v>
-      </c>
-      <c r="D118" s="11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" t="s">
-        <v>21</v>
-      </c>
-      <c r="C119" t="s">
-        <v>43</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B120" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C120" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C121" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3264,13 +3310,13 @@
         <v>13</v>
       </c>
       <c r="B122" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C122" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3281,24 +3327,24 @@
         <v>21</v>
       </c>
       <c r="C123" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C124" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3306,13 +3352,13 @@
         <v>13</v>
       </c>
       <c r="B125" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C125" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3320,27 +3366,27 @@
         <v>13</v>
       </c>
       <c r="B126" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C126" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B127" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C127" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3348,153 +3394,153 @@
         <v>13</v>
       </c>
       <c r="B128" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C128" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A129" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B129" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C129" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B130" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C130" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B131" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C131" t="s">
-        <v>32</v>
+        <v>91</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B132" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C132" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B133" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C133" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B134" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C134" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B135" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C135" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B136" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C136" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B137" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C137" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B138" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C138" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3502,41 +3548,41 @@
         <v>13</v>
       </c>
       <c r="B139" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C139" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B140" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C140" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B141" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C141" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3544,13 +3590,13 @@
         <v>13</v>
       </c>
       <c r="B142" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C142" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3558,68 +3604,166 @@
         <v>13</v>
       </c>
       <c r="B143" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" t="s">
+        <v>36</v>
+      </c>
+      <c r="D143" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A144" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B144" t="s">
         <v>22</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C144" t="s">
+        <v>92</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A145" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145" t="s">
+        <v>16</v>
+      </c>
+      <c r="C145" t="s">
+        <v>93</v>
+      </c>
+      <c r="D145" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A146" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" t="s">
+        <v>16</v>
+      </c>
+      <c r="C146" t="s">
+        <v>94</v>
+      </c>
+      <c r="D146" s="11" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A147" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" t="s">
+        <v>22</v>
+      </c>
+      <c r="C147" t="s">
+        <v>85</v>
+      </c>
+      <c r="D147" s="11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A148" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" t="s">
+        <v>22</v>
+      </c>
+      <c r="C148" t="s">
+        <v>86</v>
+      </c>
+      <c r="D148" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A149" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" t="s">
+        <v>22</v>
+      </c>
+      <c r="C149" t="s">
+        <v>87</v>
+      </c>
+      <c r="D149" s="11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A150" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B150" t="s">
+        <v>22</v>
+      </c>
+      <c r="C150" t="s">
         <v>88</v>
       </c>
-      <c r="D143" s="11" t="s">
+      <c r="D150" s="11" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A144" s="8" t="s">
+    <row r="151" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A151" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B151" t="s">
         <v>95</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C151" t="s">
         <v>96</v>
       </c>
-      <c r="D144" s="11" t="s">
+      <c r="D151" s="11" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A145" s="8" t="s">
+    <row r="152" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A152" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B152" t="s">
         <v>97</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C152" t="s">
         <v>98</v>
       </c>
-      <c r="D145" s="11" t="s">
+      <c r="D152" s="11" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A146" s="8" t="s">
+    <row r="153" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A153" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B153" t="s">
         <v>97</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C153" t="s">
         <v>99</v>
       </c>
-      <c r="D146" s="11" t="s">
+      <c r="D153" s="11" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A147" s="8" t="s">
+    <row r="154" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A154" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B154" t="s">
         <v>97</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C154" t="s">
         <v>100</v>
       </c>
-      <c r="D147" s="11" t="s">
+      <c r="D154" s="11" t="s">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v53 updates, add stnd frmwk dbplyr fixes
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/github/dqa_library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D72456-83BB-464B-9CD1-089EB51DCAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7B4F53-5CE2-CB41-ADF5-54C303D0E2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="275">
   <si>
     <t>Check Type</t>
   </si>
@@ -752,30 +752,6 @@
     <t>counts of each unique specialty_concept_id for outpatient specialties in the specialty table (visit_concept_id = 9202 when inner joined to visit_occurrence)</t>
   </si>
   <si>
-    <t>counts of concepts in procedure_concept_id that, when joined with the concept table, are not part of the following vocabularies: ICD10CM, CPT4, ICD9CM, ICD10, ICD9, ICD10PCS, ICD9Proc, HCPCS</t>
-  </si>
-  <si>
-    <t>counts of concepts in condition_source_concept_id that, when joined with the concept table, are not part of the following vocabularies: ICD9, ICD10CM, ICD10, ICD10CM</t>
-  </si>
-  <si>
-    <t>counts of concepts in imm_dose_unit_concept_id that, when joined with the concept table, are not part of the following vocabularies: UCUM</t>
-  </si>
-  <si>
-    <t>counts of concepts in cause_concept_id that, when joined with the concept table, are not part of the following vocabularies: SNOMED, OMOP Extension</t>
-  </si>
-  <si>
-    <t>counts of concepts in condition_concept_id that, when joined with the concept table, are not part of the following vocabularies: SNOMED, OMOP Extension</t>
-  </si>
-  <si>
-    <t>counts of concepts in drug_concept_id that, when joined with the concept table, are not part of the following vocabularies: RxNorm, RxNorm Extension</t>
-  </si>
-  <si>
-    <t>counts of concepts in immunization_concept_id that, when joined with the concept table, are not part of the following vocabularies: CVX</t>
-  </si>
-  <si>
-    <t>counts of concepts in dose_unit_concept_id that, when joined with the concept table, are not part of the following vocabularies: UCUM</t>
-  </si>
-  <si>
     <t>counts of concepts in service_concept_id that are not part of the list of concepts in valueset_service (found in the specs folder of the GitHub repository)</t>
   </si>
   <si>
@@ -855,6 +831,36 @@
   </si>
   <si>
     <t>counts the proportion of patients who have evidence of a drug, procedure, AND lab who also have a rapid strep lab test (ecp_concepts.csv where concept_group = rapid_strep; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>procedure_source_concept_id</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in procedure_source_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: ICD10CM, CPT4, ICD9CM, ICD10, ICD9, ICD10PCS, ICD9Proc, HCPCS</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in procedure_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: ICD10CM, CPT4, ICD9CM, ICD10, ICD9, ICD10PCS, ICD9Proc, HCPCS, SNOMED</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in condition_source_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: ICD9, ICD10CM, ICD10, ICD10CM</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in imm_dose_unit_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: UCUM</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies cause_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: SNOMED, OMOP Extension</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in condition_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: SNOMED, OMOP Extension</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in drug_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: RxNorm, RxNorm Extension</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in immunization_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: CVX</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in dose_unit_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: UCUM</t>
   </si>
 </sst>
 </file>
@@ -1001,9 +1007,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1041,7 +1047,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1147,7 +1153,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1289,7 +1295,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1297,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D157"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D46" sqref="A38:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1840,7 +1846,7 @@
         <v>59</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1848,41 +1854,41 @@
         <v>4</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>60</v>
+        <v>265</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>241</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1890,13 +1896,13 @@
         <v>4</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1904,27 +1910,27 @@
         <v>4</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>244</v>
+        <v>272</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1932,27 +1938,27 @@
         <v>4</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C46" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="D46" s="11" t="s">
-        <v>246</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1963,10 +1969,10 @@
         <v>18</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1974,13 +1980,13 @@
         <v>5</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1988,13 +1994,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2002,13 +2008,13 @@
         <v>5</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2019,24 +2025,24 @@
         <v>15</v>
       </c>
       <c r="C51" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D51" s="11" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="D52" s="11" t="s">
-        <v>141</v>
+        <v>243</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2047,10 +2053,10 @@
         <v>16</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2061,10 +2067,10 @@
         <v>16</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2075,10 +2081,10 @@
         <v>16</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2089,10 +2095,10 @@
         <v>16</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2100,30 +2106,30 @@
         <v>6</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
@@ -2131,10 +2137,10 @@
         <v>22</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2142,13 +2148,13 @@
         <v>6</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2159,10 +2165,10 @@
         <v>20</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2173,10 +2179,10 @@
         <v>20</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2184,16 +2190,16 @@
         <v>6</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>6</v>
       </c>
@@ -2201,10 +2207,10 @@
         <v>51</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2215,41 +2221,41 @@
         <v>51</v>
       </c>
       <c r="C65" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D66" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>7</v>
       </c>
@@ -2257,24 +2263,24 @@
         <v>16</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2282,13 +2288,13 @@
         <v>7</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2296,27 +2302,27 @@
         <v>7</v>
       </c>
       <c r="B71" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="C72" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="D72" s="11" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A72" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2327,24 +2333,24 @@
         <v>16</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>226</v>
+        <v>47</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2355,24 +2361,24 @@
         <v>15</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2380,55 +2386,55 @@
         <v>225</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B79" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B80" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="C80" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D79" s="11" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="D80" s="11" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2439,10 +2445,10 @@
         <v>9</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2453,13 +2459,13 @@
         <v>9</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>8</v>
       </c>
@@ -2467,13 +2473,13 @@
         <v>9</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>8</v>
       </c>
@@ -2481,13 +2487,13 @@
         <v>9</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>8</v>
       </c>
@@ -2495,13 +2501,13 @@
         <v>9</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>8</v>
       </c>
@@ -2509,10 +2515,10 @@
         <v>9</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2523,24 +2529,24 @@
         <v>9</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2551,10 +2557,10 @@
         <v>10</v>
       </c>
       <c r="C89" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2565,10 +2571,10 @@
         <v>10</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2579,10 +2585,10 @@
         <v>10</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2593,13 +2599,13 @@
         <v>10</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
         <v>8</v>
       </c>
@@ -2607,13 +2613,13 @@
         <v>10</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>8</v>
       </c>
@@ -2621,10 +2627,10 @@
         <v>10</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2635,13 +2641,13 @@
         <v>10</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>8</v>
       </c>
@@ -2649,24 +2655,24 @@
         <v>10</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>164</v>
+        <v>28</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>49</v>
+        <v>164</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2677,10 +2683,10 @@
         <v>11</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2691,10 +2697,10 @@
         <v>11</v>
       </c>
       <c r="C99" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2705,10 +2711,10 @@
         <v>11</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2719,13 +2725,13 @@
         <v>11</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>8</v>
       </c>
@@ -2733,13 +2739,13 @@
         <v>11</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>8</v>
       </c>
@@ -2747,10 +2753,10 @@
         <v>11</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2761,10 +2767,10 @@
         <v>11</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D104" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2772,13 +2778,13 @@
         <v>8</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2789,10 +2795,10 @@
         <v>12</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D106" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2803,10 +2809,10 @@
         <v>12</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2817,10 +2823,10 @@
         <v>12</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2831,13 +2837,13 @@
         <v>12</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
         <v>8</v>
       </c>
@@ -2845,13 +2851,13 @@
         <v>12</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
         <v>8</v>
       </c>
@@ -2859,10 +2865,10 @@
         <v>12</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2873,27 +2879,27 @@
         <v>12</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
-        <v>13</v>
+      <c r="A113" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C113" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
         <v>13</v>
       </c>
@@ -2901,10 +2907,10 @@
         <v>20</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2912,27 +2918,27 @@
         <v>13</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2943,10 +2949,10 @@
         <v>21</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2957,10 +2963,10 @@
         <v>21</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2971,13 +2977,13 @@
         <v>21</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>13</v>
       </c>
@@ -2985,13 +2991,13 @@
         <v>21</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>13</v>
       </c>
@@ -2999,13 +3005,13 @@
         <v>21</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
         <v>13</v>
       </c>
@@ -3013,13 +3019,13 @@
         <v>21</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>13</v>
       </c>
@@ -3027,38 +3033,38 @@
         <v>21</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3069,10 +3075,10 @@
         <v>18</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3083,10 +3089,10 @@
         <v>18</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3094,13 +3100,13 @@
         <v>13</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3111,10 +3117,10 @@
         <v>16</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3122,16 +3128,16 @@
         <v>13</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>13</v>
       </c>
@@ -3139,10 +3145,10 @@
         <v>17</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3153,10 +3159,10 @@
         <v>17</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3167,13 +3173,13 @@
         <v>17</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>13</v>
       </c>
@@ -3181,10 +3187,10 @@
         <v>17</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3195,10 +3201,10 @@
         <v>17</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3209,10 +3215,10 @@
         <v>17</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3223,10 +3229,10 @@
         <v>17</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3234,13 +3240,13 @@
         <v>13</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3248,16 +3254,16 @@
         <v>13</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>13</v>
       </c>
@@ -3265,24 +3271,24 @@
         <v>16</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3293,13 +3299,13 @@
         <v>22</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>13</v>
       </c>
@@ -3307,10 +3313,10 @@
         <v>22</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3321,38 +3327,38 @@
         <v>22</v>
       </c>
       <c r="C144" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A145" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C145" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D144" s="11" t="s">
+      <c r="D145" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A145" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C145" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A146" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B146" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3363,10 +3369,10 @@
         <v>95</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D147" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3377,136 +3383,150 @@
         <v>95</v>
       </c>
       <c r="C148" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D148" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A149" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C149" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D148" s="11" t="s">
+      <c r="D149" s="11" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A149" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="B149" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C149" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="D149" s="11" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A150" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B150" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C150" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D150" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="D150" s="11" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A151" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C151" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D151" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="D151" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A152" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C152" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D152" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="D152" s="11" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A153" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B153" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C153" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D153" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="D153" s="11" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A154" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B154" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C154" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D154" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="D154" s="11" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A155" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B155" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C155" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="D155" s="11" t="s">
         <v>261</v>
-      </c>
-      <c r="D155" s="11" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A156" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B156" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C156" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D156" s="11" t="s">
         <v>262</v>
-      </c>
-      <c r="D156" s="11" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A157" s="13" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B157" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C157" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D157" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="D157" s="11" t="s">
-        <v>272</v>
+    </row>
+    <row r="158" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A158" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C158" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="D158" s="11" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add long inpatient visit pf application
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7B4F53-5CE2-CB41-ADF5-54C303D0E2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18233D5A-F4B0-6E45-A721-6C0FCD73CC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="285">
   <si>
     <t>Check Type</t>
   </si>
@@ -861,19 +861,54 @@
   </si>
   <si>
     <t>counts of all available vocabularies in dose_unit_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: UCUM</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated procedure</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated condition</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated drug</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated procedure AND an associated drug</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated lab value</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated procedure AND an associated drug AND an associated lab value</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated record in visit_payer</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated immunization</t>
+  </si>
+  <si>
+    <t>counts of inpatient visits (visit_concept_id = 9201 or 2000000048) longer than 2 days with and without an associated ICU transfer (service_concept_id = 2000000079, 2000000080, or 2000000078)</t>
+  </si>
+  <si>
+    <t>Long Inpatient Visits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="13">
@@ -962,7 +997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -981,6 +1016,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D46" sqref="A38:D46"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98:D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2679,126 +2718,126 @@
       <c r="A98" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B98" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C98" s="11" t="s">
+      <c r="B98" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C98" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D98" s="11" t="s">
-        <v>174</v>
+      <c r="D98" s="15" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C99" s="11" t="s">
+      <c r="B99" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D99" s="11" t="s">
-        <v>175</v>
+      <c r="D99" s="15" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B100" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C100" s="11" t="s">
+      <c r="B100" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C100" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D100" s="11" t="s">
-        <v>176</v>
+      <c r="D100" s="15" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C101" s="11" t="s">
+      <c r="B101" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C101" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D101" s="11" t="s">
-        <v>177</v>
+      <c r="D101" s="15" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C102" s="11" t="s">
+      <c r="B102" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C102" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D102" s="11" t="s">
-        <v>178</v>
+      <c r="D102" s="15" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C103" s="11" t="s">
+      <c r="B103" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C103" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D103" s="11" t="s">
-        <v>179</v>
+      <c r="D103" s="15" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C104" s="11" t="s">
+      <c r="B104" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C104" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D104" s="11" t="s">
-        <v>180</v>
+      <c r="D104" s="15" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C105" s="11" t="s">
+      <c r="B105" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C105" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D105" s="11" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="D105" s="15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C106" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D106" s="11" t="s">
-        <v>182</v>
+      <c r="B106" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2806,13 +2845,13 @@
         <v>8</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D107" s="11" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2820,13 +2859,13 @@
         <v>8</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2834,13 +2873,13 @@
         <v>8</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2848,41 +2887,41 @@
         <v>8</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C110" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D110" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A111" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D110" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A111" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C111" s="11" t="s">
+      <c r="D111" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A112" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B112" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D111" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C112" s="11" t="s">
-        <v>82</v>
-      </c>
       <c r="D112" s="11" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2890,167 +2929,167 @@
         <v>8</v>
       </c>
       <c r="B113" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A114" s="7" t="s">
-        <v>13</v>
+      <c r="A114" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C114" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
-        <v>13</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>87</v>
+        <v>49</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
-        <v>13</v>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
-        <v>13</v>
+      <c r="A117" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>13</v>
+      <c r="A118" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B118" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
-        <v>13</v>
+      <c r="A119" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B119" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>13</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A120" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
-        <v>13</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A121" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B121" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
-        <v>13</v>
+      <c r="A122" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B122" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3061,10 +3100,10 @@
         <v>51</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3072,13 +3111,13 @@
         <v>13</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3086,13 +3125,13 @@
         <v>13</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3100,13 +3139,13 @@
         <v>13</v>
       </c>
       <c r="B128" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3114,27 +3153,27 @@
         <v>13</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B130" s="11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3142,139 +3181,139 @@
         <v>13</v>
       </c>
       <c r="B131" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B133" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A137" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B137" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3282,41 +3321,41 @@
         <v>13</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B142" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A143" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B143" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3324,13 +3363,13 @@
         <v>13</v>
       </c>
       <c r="B144" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3338,194 +3377,320 @@
         <v>13</v>
       </c>
       <c r="B145" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D145" s="11" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A146" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C146" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D146" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A147" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C147" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D147" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A148" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C145" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A146" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B146" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C146" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D146" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A147" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B147" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C147" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D147" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A148" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B148" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="C148" s="11" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A149" s="8" t="s">
-        <v>14</v>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A149" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>95</v>
+        <v>16</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A150" s="13" t="s">
-        <v>246</v>
+      <c r="A150" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>247</v>
+        <v>92</v>
       </c>
       <c r="D150" s="11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A151" s="13" t="s">
-        <v>246</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A151" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B151" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>248</v>
+        <v>83</v>
       </c>
       <c r="D151" s="11" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A152" s="13" t="s">
-        <v>246</v>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A152" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B152" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>249</v>
+        <v>84</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A153" s="13" t="s">
-        <v>246</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A153" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B153" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>250</v>
+        <v>85</v>
       </c>
       <c r="D153" s="11" t="s">
-        <v>259</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A154" s="13" t="s">
-        <v>246</v>
+      <c r="A154" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="B154" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C154" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D154" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A155" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C155" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D155" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A156" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C156" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D156" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A157" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C157" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D157" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A158" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C158" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D158" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A159" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C159" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A160" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B160" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C160" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D160" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A161" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C161" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A162" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C162" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A163" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C163" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="D154" s="11" t="s">
+      <c r="D163" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A155" s="13" t="s">
+    <row r="164" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A164" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="B155" s="11" t="s">
+      <c r="B164" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C155" s="11" t="s">
+      <c r="C164" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="D155" s="11" t="s">
+      <c r="D164" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A156" s="13" t="s">
+    <row r="165" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A165" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="B156" s="11" t="s">
+      <c r="B165" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C156" s="11" t="s">
+      <c r="C165" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="D156" s="11" t="s">
+      <c r="D165" s="11" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A157" s="13" t="s">
+    <row r="166" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A166" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="B157" s="11" t="s">
+      <c r="B166" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C157" s="11" t="s">
+      <c r="C166" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="D157" s="11" t="s">
+      <c r="D166" s="11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A158" s="13" t="s">
+    <row r="167" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A167" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="B158" s="11" t="s">
+      <c r="B167" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C158" s="11" t="s">
+      <c r="C167" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="D158" s="11" t="s">
+      <c r="D167" s="11" t="s">
         <v>264</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add condition_source_concept_id as uc app
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18233D5A-F4B0-6E45-A721-6C0FCD73CC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6470C50-2750-0D4C-9C6E-7549CE6A18E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="287">
   <si>
     <t>Check Type</t>
   </si>
@@ -891,6 +891,12 @@
   </si>
   <si>
     <t>Long Inpatient Visits</t>
+  </si>
+  <si>
+    <t>Condition Sources</t>
+  </si>
+  <si>
+    <t>for the full condition_occurrence table, counts of condition_source_concept_ids mapped to 44814650, 0, 44814653, or 44814649</t>
   </si>
 </sst>
 </file>
@@ -1342,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D167"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98:D106"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2172,17 +2178,17 @@
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
@@ -2190,10 +2196,10 @@
         <v>22</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2201,13 +2207,13 @@
         <v>6</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2218,10 +2224,10 @@
         <v>20</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2232,10 +2238,10 @@
         <v>20</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2243,16 +2249,16 @@
         <v>6</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>6</v>
       </c>
@@ -2260,10 +2266,10 @@
         <v>51</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2274,41 +2280,41 @@
         <v>51</v>
       </c>
       <c r="C66" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D67" s="11" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A67" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>7</v>
       </c>
@@ -2316,24 +2322,24 @@
         <v>16</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2341,13 +2347,13 @@
         <v>7</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2355,27 +2361,27 @@
         <v>7</v>
       </c>
       <c r="B72" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C73" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A73" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2386,24 +2392,24 @@
         <v>16</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>226</v>
+        <v>47</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2414,24 +2420,24 @@
         <v>15</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2439,55 +2445,55 @@
         <v>225</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="s">
         <v>225</v>
       </c>
       <c r="B80" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="B81" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="11" t="s">
+      <c r="C81" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D81" s="11" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2498,10 +2504,10 @@
         <v>9</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2512,13 +2518,13 @@
         <v>9</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>8</v>
       </c>
@@ -2526,13 +2532,13 @@
         <v>9</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>8</v>
       </c>
@@ -2540,13 +2546,13 @@
         <v>9</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>8</v>
       </c>
@@ -2554,13 +2560,13 @@
         <v>9</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>8</v>
       </c>
@@ -2568,10 +2574,10 @@
         <v>9</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2582,24 +2588,24 @@
         <v>9</v>
       </c>
       <c r="C88" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D88" s="11" t="s">
+      <c r="D89" s="11" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2610,10 +2616,10 @@
         <v>10</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2624,10 +2630,10 @@
         <v>10</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2638,10 +2644,10 @@
         <v>10</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2652,13 +2658,13 @@
         <v>10</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>8</v>
       </c>
@@ -2666,13 +2672,13 @@
         <v>10</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>8</v>
       </c>
@@ -2680,10 +2686,10 @@
         <v>10</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2694,13 +2700,13 @@
         <v>10</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
         <v>8</v>
       </c>
@@ -2708,24 +2714,24 @@
         <v>10</v>
       </c>
       <c r="C97" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A98" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="D97" s="11" t="s">
+      <c r="D98" s="11" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A98" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B98" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D98" s="15" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2736,10 +2742,10 @@
         <v>284</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2750,10 +2756,10 @@
         <v>284</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2764,10 +2770,10 @@
         <v>284</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2778,13 +2784,13 @@
         <v>284</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
         <v>8</v>
       </c>
@@ -2792,13 +2798,13 @@
         <v>284</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>8</v>
       </c>
@@ -2806,10 +2812,10 @@
         <v>284</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2820,13 +2826,13 @@
         <v>284</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D105" s="15" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
         <v>8</v>
       </c>
@@ -2834,24 +2840,24 @@
         <v>284</v>
       </c>
       <c r="C106" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A107" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="C107" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="D106" s="15" t="s">
+      <c r="D107" s="15" t="s">
         <v>283</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A107" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B107" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C107" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D107" s="11" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2862,10 +2868,10 @@
         <v>11</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2876,10 +2882,10 @@
         <v>11</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2890,10 +2896,10 @@
         <v>11</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2904,13 +2910,13 @@
         <v>11</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
         <v>8</v>
       </c>
@@ -2918,13 +2924,13 @@
         <v>11</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>8</v>
       </c>
@@ -2932,10 +2938,10 @@
         <v>11</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2946,10 +2952,10 @@
         <v>11</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2957,13 +2963,13 @@
         <v>8</v>
       </c>
       <c r="B115" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2974,10 +2980,10 @@
         <v>12</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2988,10 +2994,10 @@
         <v>12</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3002,10 +3008,10 @@
         <v>12</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3016,13 +3022,13 @@
         <v>12</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
         <v>8</v>
       </c>
@@ -3030,13 +3036,13 @@
         <v>12</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>8</v>
       </c>
@@ -3044,10 +3050,10 @@
         <v>12</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3058,27 +3064,27 @@
         <v>12</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
-        <v>13</v>
+      <c r="A123" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C123" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
         <v>13</v>
       </c>
@@ -3086,10 +3092,10 @@
         <v>20</v>
       </c>
       <c r="C124" s="11" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3097,27 +3103,27 @@
         <v>13</v>
       </c>
       <c r="B125" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3128,10 +3134,10 @@
         <v>21</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3142,10 +3148,10 @@
         <v>21</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3156,13 +3162,13 @@
         <v>21</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
         <v>13</v>
       </c>
@@ -3170,13 +3176,13 @@
         <v>21</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>13</v>
       </c>
@@ -3184,13 +3190,13 @@
         <v>21</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>13</v>
       </c>
@@ -3198,13 +3204,13 @@
         <v>21</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>13</v>
       </c>
@@ -3212,38 +3218,38 @@
         <v>21</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B134" s="11" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3254,10 +3260,10 @@
         <v>18</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3268,10 +3274,10 @@
         <v>18</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3279,13 +3285,13 @@
         <v>13</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3296,10 +3302,10 @@
         <v>16</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3307,16 +3313,16 @@
         <v>13</v>
       </c>
       <c r="B140" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A141" s="7" t="s">
         <v>13</v>
       </c>
@@ -3324,10 +3330,10 @@
         <v>17</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>207</v>
+        <v>245</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3338,10 +3344,10 @@
         <v>17</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3352,13 +3358,13 @@
         <v>17</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A144" s="7" t="s">
         <v>13</v>
       </c>
@@ -3366,10 +3372,10 @@
         <v>17</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3380,10 +3386,10 @@
         <v>17</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D145" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3394,10 +3400,10 @@
         <v>17</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3408,10 +3414,10 @@
         <v>17</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D147" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3419,13 +3425,13 @@
         <v>13</v>
       </c>
       <c r="B148" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3433,16 +3439,16 @@
         <v>13</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A150" s="7" t="s">
         <v>13</v>
       </c>
@@ -3450,24 +3456,24 @@
         <v>16</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D150" s="11" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B151" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D151" s="11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3478,13 +3484,13 @@
         <v>22</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A153" s="7" t="s">
         <v>13</v>
       </c>
@@ -3492,10 +3498,10 @@
         <v>22</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D153" s="11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3506,38 +3512,38 @@
         <v>22</v>
       </c>
       <c r="C154" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D154" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A155" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C155" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D154" s="11" t="s">
+      <c r="D155" s="11" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A155" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B155" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C155" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D155" s="11" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A156" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B156" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C156" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D156" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3548,10 +3554,10 @@
         <v>95</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3562,24 +3568,24 @@
         <v>95</v>
       </c>
       <c r="C158" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D158" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A159" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B159" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C159" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D158" s="11" t="s">
+      <c r="D159" s="11" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A159" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="B159" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C159" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="D159" s="11" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3590,13 +3596,13 @@
         <v>22</v>
       </c>
       <c r="C160" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D160" s="11" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A161" s="13" t="s">
         <v>246</v>
       </c>
@@ -3604,13 +3610,13 @@
         <v>22</v>
       </c>
       <c r="C161" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A162" s="13" t="s">
         <v>246</v>
       </c>
@@ -3618,13 +3624,13 @@
         <v>22</v>
       </c>
       <c r="C162" s="11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A163" s="13" t="s">
         <v>246</v>
       </c>
@@ -3632,13 +3638,13 @@
         <v>22</v>
       </c>
       <c r="C163" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A164" s="13" t="s">
         <v>246</v>
       </c>
@@ -3646,10 +3652,10 @@
         <v>22</v>
       </c>
       <c r="C164" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D164" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3660,10 +3666,10 @@
         <v>22</v>
       </c>
       <c r="C165" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D165" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3674,10 +3680,10 @@
         <v>22</v>
       </c>
       <c r="C166" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D166" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3688,9 +3694,23 @@
         <v>22</v>
       </c>
       <c r="C167" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D167" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A168" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C168" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="D167" s="11" t="s">
+      <c r="D168" s="11" t="s">
         <v>264</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update check metadata file
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28385F2D-6EAE-8C4A-BC9A-17FA3EF76E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5FE440-F8CD-9142-A29A-A06F2DC5FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="310">
   <si>
     <t>Check Type</t>
   </si>
@@ -897,13 +897,82 @@
   </si>
   <si>
     <t>for QUANTITATIVE lab values (labs where value_as_number is not NULL or 9999) in the measurement table, counts of unit_concept_ids mapped to 44814650, 0, 44814653, or 44814649</t>
+  </si>
+  <si>
+    <t>Influenza</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients who have evidence of a drug, procedure, AND lab who also have an influenza lab test (ecp_concepts.csv where concept_group = influenza; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>RSV</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients who have evidence of a drug, procedure, AND lab who also have an RSV lab test (ecp_concepts.csv where concept_group = rsv; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Asthma Diagnosis / Bronchodilator Drug Exposure</t>
+  </si>
+  <si>
+    <t>counts of patients with an asthma diagnosis, a bronchodilator drug exposure, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_asthma, rx_albuterol; found in the specs folder of the GitHub repository) </t>
+  </si>
+  <si>
+    <t>Condition Occurrence / Provider</t>
+  </si>
+  <si>
+    <t>Leukemia Diagnosis / Oncology Specialist</t>
+  </si>
+  <si>
+    <t>counts of patients with a leukemia diagnosis, patients who have seen an oncology specialist, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_leukemia_comb, oncology_edit; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Nephrotic Syndrome Diagnosis / Nephrology Specialist</t>
+  </si>
+  <si>
+    <t>counts of patients with a nephrotic syndrome diagnosis, patients who have seen a nephrology specialist, and patients that fall into both cohorts when the events occur within 2 years of each other (codesets: dx_nephrotic_syndrome, nephrology; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Condition Occurrence / Procedure Occurrence</t>
+  </si>
+  <si>
+    <t>Fracture Diagnosis / Imaging Procedure</t>
+  </si>
+  <si>
+    <t>counts of patients with a fracture diagnosis, an imaging procedure, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_fracture, px_radiologic; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Type 1 Diabetes Diagnosis / Insulin Drug Exposure</t>
+  </si>
+  <si>
+    <t>counts of patients with a Type 1 Diabetes diagnosis, an insulin drug exposure, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: T1D_SNOMED_codes, insulin; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Condition Occurrence / Measurement</t>
+  </si>
+  <si>
+    <t>Influenza Diagnosis / Influenza Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an Influenza diagnosis, an influenza lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_influenza, lab_influenza; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>RSV Diagnosis / RSV Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an RSV diagnosis, an RSV lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_rsv, lab_rsv; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>measurement_concept_id</t>
+  </si>
+  <si>
+    <t>counts of all available vocabularies in measurement_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: LOINC, SNOMED, PEDSnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -915,6 +984,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1003,7 +1079,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1024,6 +1100,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D168"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2007,17 +2086,17 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>68</v>
+      <c r="A47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="C47" t="s">
+        <v>308</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>237</v>
+        <v>309</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2028,10 +2107,10 @@
         <v>18</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2039,13 +2118,13 @@
         <v>5</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2053,13 +2132,13 @@
         <v>5</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2067,13 +2146,13 @@
         <v>5</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2084,24 +2163,24 @@
         <v>15</v>
       </c>
       <c r="C52" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2112,10 +2191,10 @@
         <v>16</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2126,10 +2205,10 @@
         <v>16</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2140,10 +2219,10 @@
         <v>16</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2154,10 +2233,10 @@
         <v>16</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2165,41 +2244,41 @@
         <v>6</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="14" t="s">
-        <v>284</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>285</v>
+      <c r="C59" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>142</v>
+      <c r="B60" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2210,24 +2289,24 @@
         <v>22</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>143</v>
+        <v>286</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2238,10 +2317,10 @@
         <v>20</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>77</v>
+        <v>28</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2252,10 +2331,10 @@
         <v>20</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2263,16 +2342,16 @@
         <v>6</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>6</v>
       </c>
@@ -2280,10 +2359,10 @@
         <v>51</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -2294,41 +2373,41 @@
         <v>51</v>
       </c>
       <c r="C67" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D68" s="11" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A68" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>7</v>
       </c>
@@ -2336,24 +2415,24 @@
         <v>16</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2361,13 +2440,13 @@
         <v>7</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2375,27 +2454,27 @@
         <v>7</v>
       </c>
       <c r="B73" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B74" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="C74" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D73" s="11" t="s">
+      <c r="D74" s="11" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A74" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2406,24 +2485,24 @@
         <v>16</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2434,24 +2513,24 @@
         <v>15</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2459,55 +2538,55 @@
         <v>224</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="12" t="s">
         <v>224</v>
       </c>
       <c r="B81" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B82" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C81" s="11" t="s">
+      <c r="C82" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D81" s="11" t="s">
+      <c r="D82" s="11" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2518,10 +2597,10 @@
         <v>9</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2532,13 +2611,13 @@
         <v>9</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>8</v>
       </c>
@@ -2546,13 +2625,13 @@
         <v>9</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
         <v>8</v>
       </c>
@@ -2560,13 +2639,13 @@
         <v>9</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>8</v>
       </c>
@@ -2574,13 +2653,13 @@
         <v>9</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>8</v>
       </c>
@@ -2588,10 +2667,10 @@
         <v>9</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2602,24 +2681,24 @@
         <v>9</v>
       </c>
       <c r="C89" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D90" s="11" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A90" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C90" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D90" s="11" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2630,10 +2709,10 @@
         <v>10</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2644,10 +2723,10 @@
         <v>10</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2658,10 +2737,10 @@
         <v>10</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2672,13 +2751,13 @@
         <v>10</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
         <v>8</v>
       </c>
@@ -2686,13 +2765,13 @@
         <v>10</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
         <v>8</v>
       </c>
@@ -2700,10 +2779,10 @@
         <v>10</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2714,13 +2793,13 @@
         <v>10</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>8</v>
       </c>
@@ -2728,24 +2807,24 @@
         <v>10</v>
       </c>
       <c r="C98" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="D98" s="11" t="s">
+      <c r="D99" s="11" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B99" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D99" s="15" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2756,10 +2835,10 @@
         <v>283</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2770,10 +2849,10 @@
         <v>283</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D101" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2784,10 +2863,10 @@
         <v>283</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D102" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2798,13 +2877,13 @@
         <v>283</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
         <v>8</v>
       </c>
@@ -2812,13 +2891,13 @@
         <v>283</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
         <v>8</v>
       </c>
@@ -2826,10 +2905,10 @@
         <v>283</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D105" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2840,13 +2919,13 @@
         <v>283</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
         <v>8</v>
       </c>
@@ -2854,24 +2933,24 @@
         <v>283</v>
       </c>
       <c r="C107" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A108" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="C108" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D108" s="15" t="s">
         <v>282</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A108" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C108" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D108" s="11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2882,10 +2961,10 @@
         <v>11</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D109" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2896,10 +2975,10 @@
         <v>11</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2910,10 +2989,10 @@
         <v>11</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2924,13 +3003,13 @@
         <v>11</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
         <v>8</v>
       </c>
@@ -2938,13 +3017,13 @@
         <v>11</v>
       </c>
       <c r="C113" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
         <v>8</v>
       </c>
@@ -2952,10 +3031,10 @@
         <v>11</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2966,10 +3045,10 @@
         <v>11</v>
       </c>
       <c r="C115" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D115" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2977,13 +3056,13 @@
         <v>8</v>
       </c>
       <c r="B116" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C116" s="11" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D116" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2994,10 +3073,10 @@
         <v>12</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3008,10 +3087,10 @@
         <v>12</v>
       </c>
       <c r="C118" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3022,10 +3101,10 @@
         <v>12</v>
       </c>
       <c r="C119" s="11" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3036,13 +3115,13 @@
         <v>12</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
         <v>8</v>
       </c>
@@ -3050,13 +3129,13 @@
         <v>12</v>
       </c>
       <c r="C121" s="11" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
         <v>8</v>
       </c>
@@ -3064,10 +3143,10 @@
         <v>12</v>
       </c>
       <c r="C122" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3078,27 +3157,27 @@
         <v>12</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A124" s="7" t="s">
-        <v>13</v>
+      <c r="A124" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B124" s="11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C124" s="11" t="s">
         <v>28</v>
       </c>
       <c r="D124" s="11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
         <v>13</v>
       </c>
@@ -3106,10 +3185,10 @@
         <v>20</v>
       </c>
       <c r="C125" s="11" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="D125" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3117,27 +3196,27 @@
         <v>13</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B127" s="11" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C127" s="11" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="D127" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3148,10 +3227,10 @@
         <v>21</v>
       </c>
       <c r="C128" s="11" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D128" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3162,10 +3241,10 @@
         <v>21</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3176,13 +3255,13 @@
         <v>21</v>
       </c>
       <c r="C130" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" s="7" t="s">
         <v>13</v>
       </c>
@@ -3190,13 +3269,13 @@
         <v>21</v>
       </c>
       <c r="C131" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D131" s="11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
         <v>13</v>
       </c>
@@ -3204,13 +3283,13 @@
         <v>21</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A133" s="7" t="s">
         <v>13</v>
       </c>
@@ -3218,13 +3297,13 @@
         <v>21</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="D133" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
         <v>13</v>
       </c>
@@ -3232,38 +3311,38 @@
         <v>21</v>
       </c>
       <c r="C134" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A135" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B136" s="11" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C136" s="11" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3274,10 +3353,10 @@
         <v>18</v>
       </c>
       <c r="C137" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3288,10 +3367,10 @@
         <v>18</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3299,13 +3378,13 @@
         <v>13</v>
       </c>
       <c r="B139" s="11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C139" s="11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3316,10 +3395,10 @@
         <v>16</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="141" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3327,16 +3406,16 @@
         <v>13</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A142" s="7" t="s">
         <v>13</v>
       </c>
@@ -3344,10 +3423,10 @@
         <v>17</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>206</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3358,10 +3437,10 @@
         <v>17</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D143" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3372,13 +3451,13 @@
         <v>17</v>
       </c>
       <c r="C144" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D144" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A145" s="7" t="s">
         <v>13</v>
       </c>
@@ -3386,10 +3465,10 @@
         <v>17</v>
       </c>
       <c r="C145" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D145" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3400,10 +3479,10 @@
         <v>17</v>
       </c>
       <c r="C146" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D146" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3414,10 +3493,10 @@
         <v>17</v>
       </c>
       <c r="C147" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D147" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3428,10 +3507,10 @@
         <v>17</v>
       </c>
       <c r="C148" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3439,13 +3518,13 @@
         <v>13</v>
       </c>
       <c r="B149" s="11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C149" s="11" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3453,16 +3532,16 @@
         <v>13</v>
       </c>
       <c r="B150" s="11" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C150" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D150" s="11" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A151" s="7" t="s">
         <v>13</v>
       </c>
@@ -3470,24 +3549,24 @@
         <v>16</v>
       </c>
       <c r="C151" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D151" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A152" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B152" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C152" s="11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -3498,13 +3577,13 @@
         <v>22</v>
       </c>
       <c r="C153" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D153" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A154" s="7" t="s">
         <v>13</v>
       </c>
@@ -3512,10 +3591,10 @@
         <v>22</v>
       </c>
       <c r="C154" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D154" s="11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3526,178 +3605,178 @@
         <v>22</v>
       </c>
       <c r="C155" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D155" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A156" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C156" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D155" s="11" t="s">
+      <c r="D156" s="11" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A156" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B156" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C156" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="D156" s="11" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A157" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B157" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C157" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A158" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C158" s="11" t="s">
-        <v>97</v>
+      <c r="B158" t="s">
+        <v>93</v>
+      </c>
+      <c r="C158" t="s">
+        <v>291</v>
       </c>
       <c r="D158" s="11" t="s">
-        <v>221</v>
+        <v>292</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A159" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B159" s="11" t="s">
+      <c r="B159" t="s">
+        <v>293</v>
+      </c>
+      <c r="C159" t="s">
+        <v>294</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A160" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B160" t="s">
+        <v>293</v>
+      </c>
+      <c r="C160" t="s">
+        <v>296</v>
+      </c>
+      <c r="D160" s="11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A161" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B161" t="s">
+        <v>298</v>
+      </c>
+      <c r="C161" t="s">
+        <v>299</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A162" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B162" t="s">
+        <v>93</v>
+      </c>
+      <c r="C162" t="s">
+        <v>301</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A163" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B163" t="s">
+        <v>303</v>
+      </c>
+      <c r="C163" t="s">
+        <v>304</v>
+      </c>
+      <c r="D163" s="11" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A164" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B164" t="s">
+        <v>303</v>
+      </c>
+      <c r="C164" t="s">
+        <v>306</v>
+      </c>
+      <c r="D164" s="11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A165" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C159" s="11" t="s">
+      <c r="C165" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D165" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A166" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B166" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C166" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D166" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A167" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B167" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C167" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D159" s="11" t="s">
+      <c r="D167" s="11" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A160" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B160" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C160" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D160" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A161" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C161" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="D161" s="11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A162" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C162" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="D162" s="11" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A163" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B163" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C163" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="D163" s="11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A164" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B164" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C164" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="D164" s="11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A165" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B165" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>251</v>
-      </c>
-      <c r="D165" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A166" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B166" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C166" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="D166" s="11" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A167" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B167" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C167" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="D167" s="11" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3708,10 +3787,150 @@
         <v>22</v>
       </c>
       <c r="C168" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D168" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A169" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C169" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D169" s="11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A170" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B170" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C170" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="D170" s="11" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A171" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B171" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C171" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="D171" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A172" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B172" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C172" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="D172" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A173" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B173" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C173" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D173" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A174" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B174" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C174" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="D174" s="11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A175" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B175" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C175" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="D175" s="11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A176" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B176" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C176" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="D168" s="11" t="s">
+      <c r="D176" s="11" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A177" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B177" t="s">
+        <v>22</v>
+      </c>
+      <c r="C177" t="s">
+        <v>287</v>
+      </c>
+      <c r="D177" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A178" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B178" t="s">
+        <v>22</v>
+      </c>
+      <c r="C178" t="s">
+        <v>289</v>
+      </c>
+      <c r="D178" s="16" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
shrink time window for flu/rsv dcon, look for prov or cs spec in dcon
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5FE440-F8CD-9142-A29A-A06F2DC5FA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF6F303-7155-DA4C-B30B-463313740D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="820" windowWidth="26700" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
+    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="314">
   <si>
     <t>Check Type</t>
   </si>
@@ -950,22 +950,34 @@
     <t>Condition Occurrence / Measurement</t>
   </si>
   <si>
-    <t>Influenza Diagnosis / Influenza Lab Test</t>
-  </si>
-  <si>
-    <t>counts of patients with an Influenza diagnosis, an influenza lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_influenza, lab_influenza; found in the specs folder of the GitHub repository)</t>
-  </si>
-  <si>
-    <t>RSV Diagnosis / RSV Lab Test</t>
-  </si>
-  <si>
-    <t>counts of patients with an RSV diagnosis, an RSV lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_rsv, lab_rsv; found in the specs folder of the GitHub repository)</t>
-  </si>
-  <si>
     <t>measurement_concept_id</t>
   </si>
   <si>
     <t>counts of all available vocabularies in measurement_concept_id, flagging when the vocabulary is not conformant to the acceptable values of: LOINC, SNOMED, PEDSnet</t>
+  </si>
+  <si>
+    <t>Influenza Diagnosis / Positive Influenza Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an Influenza diagnosis, a positive influenza lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_influenza, lab_influenza; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>Influenza Diagnosis / Negative Influenza Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an Influenza diagnosis, a negative influenza lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_influenza, lab_influenza; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>RSV Diagnosis / RSV Positive Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an RSV diagnosis, a positive RSV lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_rsv, lab_rsv; found in the specs folder of the GitHub repository)</t>
+  </si>
+  <si>
+    <t>RSV Diagnosis / RSV Negative Lab Test</t>
+  </si>
+  <si>
+    <t>counts of patients with an RSV diagnosis, a negative RSV lab test, and patients that fall into both cohorts when the events occur within 3 months of each other (codesets: dx_rsv, lab_rsv; found in the specs folder of the GitHub repository)</t>
   </si>
 </sst>
 </file>
@@ -1427,10 +1439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2093,10 +2105,10 @@
         <v>30</v>
       </c>
       <c r="C47" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3717,10 +3729,10 @@
         <v>303</v>
       </c>
       <c r="C163" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3731,38 +3743,38 @@
         <v>303</v>
       </c>
       <c r="C164" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D164" s="11" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A165" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B165" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C165" s="11" t="s">
-        <v>96</v>
+      <c r="B165" t="s">
+        <v>303</v>
+      </c>
+      <c r="C165" t="s">
+        <v>310</v>
       </c>
       <c r="D165" s="11" t="s">
-        <v>222</v>
+        <v>311</v>
       </c>
     </row>
     <row r="166" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A166" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B166" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C166" s="11" t="s">
-        <v>97</v>
+      <c r="B166" t="s">
+        <v>303</v>
+      </c>
+      <c r="C166" t="s">
+        <v>312</v>
       </c>
       <c r="D166" s="11" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3773,41 +3785,41 @@
         <v>95</v>
       </c>
       <c r="C167" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D167" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A168" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B168" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C168" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D168" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A169" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C169" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D167" s="11" t="s">
+      <c r="D169" s="11" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A168" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B168" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C168" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="D168" s="11" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" ht="68" x14ac:dyDescent="0.2">
-      <c r="A169" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C169" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="D169" s="11" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A170" s="13" t="s">
         <v>245</v>
       </c>
@@ -3815,10 +3827,10 @@
         <v>22</v>
       </c>
       <c r="C170" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D170" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3829,10 +3841,10 @@
         <v>22</v>
       </c>
       <c r="C171" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D171" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -3843,10 +3855,10 @@
         <v>22</v>
       </c>
       <c r="C172" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D172" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3857,13 +3869,13 @@
         <v>22</v>
       </c>
       <c r="C173" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D173" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A174" s="13" t="s">
         <v>245</v>
       </c>
@@ -3871,10 +3883,10 @@
         <v>22</v>
       </c>
       <c r="C174" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D174" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3885,10 +3897,10 @@
         <v>22</v>
       </c>
       <c r="C175" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D175" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -3899,37 +3911,65 @@
         <v>22</v>
       </c>
       <c r="C176" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D176" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="177" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A177" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B177" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C177" t="s">
-        <v>287</v>
+      <c r="C177" s="11" t="s">
+        <v>253</v>
       </c>
       <c r="D177" s="11" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A178" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B178" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C178" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D178" s="11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A179" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B179" t="s">
+        <v>22</v>
+      </c>
+      <c r="C179" t="s">
+        <v>287</v>
+      </c>
+      <c r="D179" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A180" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B180" t="s">
+        <v>22</v>
+      </c>
+      <c r="C180" t="s">
         <v>289</v>
       </c>
-      <c r="D178" s="16" t="s">
+      <c r="D180" s="16" t="s">
         <v>290</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add new geocode checks to description, add license
</commit_message>
<xml_diff>
--- a/dqa_check_descriptions.xlsx
+++ b/dqa_check_descriptions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wieandk/Desktop/data_quality/dqa_library/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AED2E-C14E-914B-AA8E-C733782A2323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7C47C0-9DC4-B946-8B4D-B4EFF149768F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="2100" windowWidth="25800" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
+    <workbookView xWindow="4440" yWindow="820" windowWidth="25800" windowHeight="17360" xr2:uid="{EA2FCE8C-5E9B-744D-8FD9-489DF3342686}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="340">
   <si>
     <t>Check Type</t>
   </si>
@@ -998,27 +998,15 @@
     <t>Census Tract Geocode (2010)</t>
   </si>
   <si>
-    <t>counts the proportion of ALL patients have a valid, 11-digit tract level geocode for the 2010 census year associated with their current location (location_id in the person table)</t>
-  </si>
-  <si>
     <t>Census Tract Geocode (2020)</t>
   </si>
   <si>
-    <t>counts the proportion of ALL patients have a valid, 11-digit tract level geocode for the 2020 census year associated with their current location (location_id in the person table)</t>
-  </si>
-  <si>
     <t>Census Block Group Geocode (2010)</t>
   </si>
   <si>
-    <t>counts the proportion of ALL patients have a valid, 12-digit block group level geocode for the 2010 census year associated with their current location (location_id in the person table)</t>
-  </si>
-  <si>
     <t>Census Block Group Geocode (2020)</t>
   </si>
   <si>
-    <t>counts the proportion of ALL patients have a valid, 12-digit block group level geocode for the 2020 census year associated with their current location (location_id in the person table)</t>
-  </si>
-  <si>
     <t>Census Tract Geocode</t>
   </si>
   <si>
@@ -1029,6 +1017,45 @@
   </si>
   <si>
     <t>counts of each distinct length of a census tract level geocode, removing NULL values and invalid characters (ideally is 12 digits)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have have a valid, 11-digit tract level geocode for the 2010 census year associated with their current location (location_id in the person table)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 11-digit tract level geocode for the 2020 census year associated with their current location (location_id in the person table)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 12-digit block group level geocode for the 2010 census year associated with their current location (location_id in the person table)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 12-digit block group level geocode for the 2020 census year associated with their current location (location_id in the person table)</t>
+  </si>
+  <si>
+    <t>Location History</t>
+  </si>
+  <si>
+    <t>2+ Census Tract Location History Geocodes (2010)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 11-digit tract level geocode for the 2010 census associated with MORE THAN ONE location in the location_history table</t>
+  </si>
+  <si>
+    <t>2+ Census Tract Location History Geocodes (2020)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 11-digit tract level geocode for the 2020 census associated with MORE THAN ONE location in the location_history table</t>
+  </si>
+  <si>
+    <t>2+ Census Block Group Location History Geocodes (2010)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 12-digit block group level geocode for the 2010 census associated with MORE THAN ONE location in the location_history table</t>
+  </si>
+  <si>
+    <t>2+ Census Block Group Location History Geocodes (2020)</t>
+  </si>
+  <si>
+    <t>counts the proportion of patients with a valid sex, DOB, and at least 1 diagnosis associated with a FTF visit that also have a valid, 12-digit block group level geocode for the 2020 census associated with MORE THAN ONE location in the location_history table</t>
   </si>
 </sst>
 </file>
@@ -1501,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7874EDB4-381F-6540-806F-73BCCBEA88CA}">
-  <dimension ref="A1:D189"/>
+  <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82:D83"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2657,10 +2684,10 @@
         <v>318</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -2671,10 +2698,10 @@
         <v>318</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4105,60 +4132,116 @@
         <v>317</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A186" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="B186" s="17" t="s">
+      <c r="B186" t="s">
         <v>318</v>
       </c>
-      <c r="C186" s="17" t="s">
+      <c r="C186" t="s">
         <v>319</v>
       </c>
-      <c r="D186" s="18" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="D186" s="11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A187" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="B187" s="17" t="s">
+      <c r="B187" t="s">
         <v>318</v>
       </c>
-      <c r="C187" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="D187" s="18" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="C187" t="s">
+        <v>320</v>
+      </c>
+      <c r="D187" s="11" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A188" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="B188" s="17" t="s">
+      <c r="B188" t="s">
         <v>318</v>
       </c>
-      <c r="C188" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="D188" s="18" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="C188" t="s">
+        <v>321</v>
+      </c>
+      <c r="D188" s="11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A189" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="B189" s="17" t="s">
+      <c r="B189" t="s">
         <v>318</v>
       </c>
-      <c r="C189" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="D189" s="18" t="s">
-        <v>326</v>
+      <c r="C189" t="s">
+        <v>322</v>
+      </c>
+      <c r="D189" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A190" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B190" t="s">
+        <v>331</v>
+      </c>
+      <c r="C190" t="s">
+        <v>332</v>
+      </c>
+      <c r="D190" s="11" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A191" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B191" t="s">
+        <v>331</v>
+      </c>
+      <c r="C191" t="s">
+        <v>334</v>
+      </c>
+      <c r="D191" s="11" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A192" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B192" t="s">
+        <v>331</v>
+      </c>
+      <c r="C192" t="s">
+        <v>336</v>
+      </c>
+      <c r="D192" s="11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A193" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="B193" t="s">
+        <v>331</v>
+      </c>
+      <c r="C193" t="s">
+        <v>338</v>
+      </c>
+      <c r="D193" s="11" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>